<commit_message>
Allowing queing for metadata runs
</commit_message>
<xml_diff>
--- a/activity_overrides.xlsx
+++ b/activity_overrides.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H517"/>
+  <dimension ref="A1:H518"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13409,6 +13409,28 @@
         </is>
       </c>
     </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>2026-02-07 #1</t>
+        </is>
+      </c>
+      <c r="B518" t="n">
+        <v>0</v>
+      </c>
+      <c r="C518" t="n">
+        <v>0</v>
+      </c>
+      <c r="D518" t="inlineStr"/>
+      <c r="E518" t="inlineStr"/>
+      <c r="F518" t="inlineStr"/>
+      <c r="G518" t="inlineStr"/>
+      <c r="H518" t="inlineStr">
+        <is>
+          <t>Warmup</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Tidy up metadata screen
</commit_message>
<xml_diff>
--- a/activity_overrides.xlsx
+++ b/activity_overrides.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul.collyer\Dropbox\Running and Cycling\DataPipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B0047E-C9CD-4AB8-9151-A9B656383CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CF549B-47C2-44EB-A171-B899D91B9963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3340,13 +3340,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H516"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A473" workbookViewId="0">
-      <selection activeCell="H523" sqref="H523"/>
+    <sheetView tabSelected="1" topLeftCell="A502" workbookViewId="0">
+      <selection activeCell="A502" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>